<commit_message>
update note on Stack Frame
</commit_message>
<xml_diff>
--- a/26_AssemblyLanguage_And_Storage/Stack Frame.xlsx
+++ b/26_AssemblyLanguage_And_Storage/Stack Frame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\Computer\C-Code\26_AssemblyLanguage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\Computer\C-Code\26_AssemblyLanguage_And_Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88D1390-68F0-4538-904E-565C7D326048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B0883C-3047-4F9F-AF04-249257B60CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="309" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="309" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="函数调用分析" sheetId="2" r:id="rId1"/>
@@ -781,6 +781,36 @@
           <a:r>
             <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
             <a:t>具体在函数调用时的变化没有理解，后期待研究。</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" altLang="zh-CN" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>注：</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" altLang="zh-CN" sz="1100"/>
+            <a:t>%</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>rbp</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>固定指向栈底部，</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" altLang="zh-CN" sz="1100"/>
+            <a:t>%rsp</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+            <a:t>指向栈顶部且随着入栈而变化</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
@@ -2084,8 +2114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA8C85-79A6-4A22-9D08-55E58E08DFDF}">
   <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2324,7 +2354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C4:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update note about stack
</commit_message>
<xml_diff>
--- a/26_AssemblyLanguage_And_Storage/Stack Frame.xlsx
+++ b/26_AssemblyLanguage_And_Storage/Stack Frame.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\Computer\C-Code\26_AssemblyLanguage_And_Storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880DCE29-97A8-45D5-AF1B-67BEC17DF7E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF7FBEE-1F44-4305-97B8-79552723E74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="309" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>0xfe100</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>foo()</t>
-  </si>
-  <si>
-    <t>x64系统中每次移动8位</t>
   </si>
   <si>
     <t>2(%edi)</t>
@@ -123,23 +120,29 @@
   <si>
     <t>对应代码"\2_C_and_Assembly\coursework\DebugTest.c"</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>x64系统中每次移动8位(8bytes x 8 = 64 bits)</t>
+  </si>
+  <si>
+    <t>即地址都是用64bits表示的。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -147,13 +150,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -238,7 +241,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2122,26 +2125,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA8C85-79A6-4A22-9D08-55E58E08DFDF}">
   <dimension ref="B1:O47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="6" width="9.125" customWidth="1"/>
-    <col min="8" max="8" width="14.25" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:15" ht="43.5" customHeight="1">
       <c r="F1" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:15">
       <c r="F3" t="s">
         <v>1</v>
       </c>
@@ -2162,7 +2165,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:15">
       <c r="B4" s="5"/>
       <c r="C4" t="s">
         <v>5</v>
@@ -2183,7 +2186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:15">
       <c r="B5" s="4"/>
       <c r="C5" t="s">
         <v>20</v>
@@ -2198,7 +2201,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:15">
       <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2209,7 +2212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:15">
       <c r="F7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2217,27 +2220,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:15">
       <c r="F8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15">
       <c r="F9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:15">
       <c r="F10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15">
       <c r="F11" s="2">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15">
       <c r="F12" s="2">
         <v>108</v>
       </c>
@@ -2248,45 +2251,48 @@
         <v>20</v>
       </c>
       <c r="K12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
       <c r="F13" s="2">
         <v>107</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
       <c r="F14" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15">
       <c r="F15" s="2">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:15">
       <c r="F16" s="2">
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:9">
       <c r="F17" s="2">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:9">
       <c r="F18" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:9">
       <c r="F19" s="2">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:9">
       <c r="F20" t="s">
         <v>0</v>
       </c>
@@ -2297,55 +2303,55 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="6:9">
       <c r="F24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="6:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="6:9">
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="6:9">
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="6:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="6:9">
       <c r="G27" s="7"/>
     </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="6:7">
       <c r="F40" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7">
+      <c r="G41" s="7"/>
+    </row>
+    <row r="42" spans="6:7">
+      <c r="G42" s="7"/>
+    </row>
+    <row r="43" spans="6:7">
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="6:7">
+      <c r="F44" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G44" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G41" s="7"/>
-    </row>
-    <row r="42" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G42" s="7"/>
-    </row>
-    <row r="43" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="G43" s="7"/>
-    </row>
-    <row r="44" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F44" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="6:7">
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="6:7">
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="6:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="6:7">
       <c r="G47" s="7"/>
     </row>
   </sheetData>
@@ -2370,168 +2376,168 @@
       <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="12.875" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.75" customWidth="1"/>
-    <col min="11" max="11" width="21.625" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:9">
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:9">
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:9">
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:9">
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:9">
       <c r="C8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:9">
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:9">
       <c r="C10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:9">
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:9">
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:9">
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:9">
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:9">
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:9">
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:8">
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:8">
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:8">
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:8">
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:8">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:8">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:8">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:8">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:8">
       <c r="C25" s="1"/>
       <c r="G25" s="9"/>
       <c r="H25" s="3"/>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:8">
       <c r="C26" s="1"/>
       <c r="G26" s="9"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:8">
       <c r="C27" s="1"/>
       <c r="G27" s="9"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:8">
       <c r="G28" s="9"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:8">
       <c r="G29" s="9"/>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:8">
       <c r="G30" s="10"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:8">
       <c r="G31" s="10"/>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:8">
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="7:7">
       <c r="G33" s="10"/>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="6:6">
       <c r="F61" s="3"/>
     </row>
-    <row r="77" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="6:8">
       <c r="F77" s="3"/>
       <c r="G77" s="10"/>
       <c r="H77" s="3"/>
     </row>
-    <row r="78" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="6:8">
       <c r="G78" s="10"/>
     </row>
-    <row r="79" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="6:8">
       <c r="G79" s="10"/>
     </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="6:8">
       <c r="G80" s="10"/>
     </row>
-    <row r="81" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="6:8">
       <c r="F81" s="3"/>
       <c r="G81" s="10"/>
       <c r="H81" s="3"/>
     </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="6:8">
       <c r="G82" s="10"/>
     </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="6:8">
       <c r="G83" s="10"/>
     </row>
-    <row r="84" spans="6:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="6:8">
       <c r="G84" s="10"/>
     </row>
   </sheetData>

</xml_diff>